<commit_message>
update excel test cases
</commit_message>
<xml_diff>
--- a/2018_7/Q1/exe/result.xlsx
+++ b/2018_7/Q1/exe/result.xlsx
@@ -7,9 +7,13 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20180708_190629" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20180708_190410" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20180708_211007" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20180708_210523" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20180708_210410" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20180708_205948" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20180708_190629" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20180708_190410" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>Index</t>
   </si>
@@ -46,22 +50,58 @@
     <t>10</t>
   </si>
   <si>
+    <t>391</t>
+  </si>
+  <si>
+    <t>Passed:1Wrong:5</t>
+  </si>
+  <si>
+    <t>find_diff_Felix_py3.py</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>387</t>
+  </si>
+  <si>
+    <t>All 6 cases passed!</t>
+  </si>
+  <si>
+    <t>394</t>
+  </si>
+  <si>
+    <t>379</t>
+  </si>
+  <si>
+    <t>381</t>
+  </si>
+  <si>
+    <t>380</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>515</t>
+  </si>
+  <si>
+    <t>Wrong:2</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>385</t>
+  </si>
+  <si>
+    <t>All 2 cases passed!</t>
+  </si>
+  <si>
     <t>406</t>
   </si>
   <si>
-    <t>Passed:1Wrong:5</t>
-  </si>
-  <si>
-    <t>find_diff_Felix_py3.py</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
     <t>414</t>
-  </si>
-  <si>
-    <t>All 6 cases passed!</t>
   </si>
   <si>
     <t>420</t>
@@ -418,6 +458,354 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
+    <col customWidth="1" max="1" min="1" width="10"/>
+    <col customWidth="1" max="2" min="2" width="50"/>
+    <col customWidth="1" max="3" min="3" width="10"/>
+    <col customWidth="1" max="4" min="4" width="10"/>
+    <col customWidth="1" max="5" min="5" width="10"/>
+    <col customWidth="1" max="6" min="6" width="50"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="10"/>
+    <col customWidth="1" max="2" min="2" width="50"/>
+    <col customWidth="1" max="3" min="3" width="10"/>
+    <col customWidth="1" max="4" min="4" width="10"/>
+    <col customWidth="1" max="5" min="5" width="10"/>
+    <col customWidth="1" max="6" min="6" width="50"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="10"/>
+    <col customWidth="1" max="2" min="2" width="50"/>
+    <col customWidth="1" max="3" min="3" width="10"/>
+    <col customWidth="1" max="4" min="4" width="10"/>
+    <col customWidth="1" max="5" min="5" width="10"/>
+    <col customWidth="1" max="6" min="6" width="50"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="10"/>
+    <col customWidth="1" max="2" min="2" width="50"/>
+    <col customWidth="1" max="3" min="3" width="10"/>
+    <col customWidth="1" max="4" min="4" width="10"/>
+    <col customWidth="1" max="5" min="5" width="10"/>
+    <col customWidth="1" max="6" min="6" width="50"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
     <col customWidth="1" max="1" min="1" width="15"/>
     <col customWidth="1" max="2" min="2" width="50"/>
     <col customWidth="1" max="3" min="3" width="15"/>
@@ -460,7 +848,7 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -480,7 +868,7 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
@@ -491,7 +879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -547,7 +935,7 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -567,7 +955,7 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
@@ -578,7 +966,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>